<commit_message>
All data in Excel sheet and first graphs in report
</commit_message>
<xml_diff>
--- a/matlab/Histograms.xlsx
+++ b/matlab/Histograms.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Metric 1</t>
   </si>
@@ -94,6 +94,30 @@
   <si>
     <t>ϑ=5 n=30 s=-1/+1</t>
   </si>
+  <si>
+    <t>1-Mean</t>
+  </si>
+  <si>
+    <t>Public</t>
+  </si>
+  <si>
+    <t>No adaptation</t>
+  </si>
+  <si>
+    <t>Adaptive</t>
+  </si>
+  <si>
+    <t>alpha =1 beta = 0,1 minR=0,2 maxR=0,4</t>
+  </si>
+  <si>
+    <t>alpha =1 beta = 0,2 minR=0,2 maxR=0,4</t>
+  </si>
+  <si>
+    <t>alpha =1 beta = 0,2 minR=0,06 maxR=0,4</t>
+  </si>
+  <si>
+    <t>alpha =1 beta = 0,1 minR=0,06 maxR=0,4</t>
+  </si>
 </sst>
 </file>
 
@@ -153,7 +177,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -196,21 +220,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -329,30 +338,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -380,6 +365,46 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -387,6 +412,109 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -401,63 +529,107 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20 % - Accent1" xfId="2" builtinId="30"/>
@@ -492,77 +664,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Fixed</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> thresholds</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Metric 1</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -574,7 +676,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$E$5</c:f>
+              <c:f>Feuil1!$F$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -599,7 +701,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Feuil1!$F$6:$F$11</c:f>
+                <c:f>Feuil1!$G$6:$G$11</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
@@ -626,7 +728,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Feuil1!$F$6:$F$11</c:f>
+                <c:f>Feuil1!$G$6:$G$11</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
@@ -666,34 +768,35 @@
             </c:spPr>
           </c:errBars>
           <c:cat>
-            <c:strRef>
-              <c:f>Feuil1!$D$6:$D$11</c:f>
-              <c:strCache>
+            <c:numRef>
+              <c:f>Feuil1!$E$6:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>ϑ=5 n=INF</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>ϑ=8 n=INF</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>ϑ=5 n=10</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>ϑ=8 n=10</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>ϑ=5 n=30</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>ϑ=8 n=30</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$E$6:$E$11</c:f>
+              <c:f>Feuil1!$F$6:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -729,11 +832,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="210228624"/>
-        <c:axId val="210236784"/>
+        <c:axId val="-849458496"/>
+        <c:axId val="-849460672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="210228624"/>
+        <c:axId val="-849458496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -761,7 +864,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -776,17 +879,18 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210236784"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="-849460672"/>
+        <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210236784"/>
+        <c:axId val="-849460672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="5.000000000000001E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -820,7 +924,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -835,9 +939,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210228624"/>
+        <c:crossAx val="-849458496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="5.000000000000001E-2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -975,7 +1080,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$G$5</c:f>
+              <c:f>Feuil1!$H$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1000,7 +1105,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Feuil1!$H$6:$H$11</c:f>
+                <c:f>Feuil1!$J$6:$J$11</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
@@ -1027,7 +1132,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Feuil1!$H$6:$H$11</c:f>
+                <c:f>Feuil1!$J$6:$J$11</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
@@ -1094,27 +1199,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$G$6:$G$11</c:f>
+              <c:f>Feuil1!$I$6:$I$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.40652814999999998</c:v>
+                  <c:v>0.59347185000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.30257622499999998</c:v>
+                  <c:v>0.69742377500000008</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.43228597499999999</c:v>
+                  <c:v>0.56771402500000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.39777544999999997</c:v>
+                  <c:v>0.60222455000000008</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.48667115</c:v>
+                  <c:v>0.51332884999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.33149679999999998</c:v>
+                  <c:v>0.66850319999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1130,11 +1235,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="210229712"/>
-        <c:axId val="210230256"/>
+        <c:axId val="-849466112"/>
+        <c:axId val="-849461216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="210229712"/>
+        <c:axId val="-849466112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1177,7 +1282,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210230256"/>
+        <c:crossAx val="-849461216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1185,7 +1290,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210230256"/>
+        <c:axId val="-849461216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1236,7 +1341,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210229712"/>
+        <c:crossAx val="-849466112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1381,7 +1486,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$E$5</c:f>
+              <c:f>Feuil1!$F$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1406,7 +1511,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Feuil1!$F$12:$F$15</c:f>
+                <c:f>Feuil1!$G$12:$G$15</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
@@ -1427,7 +1532,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Feuil1!$F$12:$F$15</c:f>
+                <c:f>Feuil1!$G$12:$G$15</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
@@ -1482,7 +1587,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$E$12:$E$15</c:f>
+              <c:f>Feuil1!$F$12:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1512,11 +1617,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="531371200"/>
-        <c:axId val="531370656"/>
+        <c:axId val="-849454688"/>
+        <c:axId val="-849457408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="531371200"/>
+        <c:axId val="-849454688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1559,7 +1664,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="531370656"/>
+        <c:crossAx val="-849457408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1567,9 +1672,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="531370656"/>
+        <c:axId val="-849457408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.15000000000000002"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1618,7 +1724,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="531371200"/>
+        <c:crossAx val="-849454688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1758,7 +1864,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$G$5</c:f>
+              <c:f>Feuil1!$H$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1783,7 +1889,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Feuil1!$H$12:$H$15</c:f>
+                <c:f>Feuil1!$J$12:$J$15</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
@@ -1804,7 +1910,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Feuil1!$H$12:$H$15</c:f>
+                <c:f>Feuil1!$J$12:$J$15</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
@@ -1859,21 +1965,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$G$12:$G$15</c:f>
+              <c:f>Feuil1!$I$12:$I$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.66134327500000001</c:v>
+                  <c:v>0.33865672499999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.49064137499999999</c:v>
+                  <c:v>0.50935862499999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.66827780000000003</c:v>
+                  <c:v>0.33172219999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.47091192500000001</c:v>
+                  <c:v>0.52908807499999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1889,11 +1995,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="531385344"/>
-        <c:axId val="531379904"/>
+        <c:axId val="-849456320"/>
+        <c:axId val="-849463392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="531385344"/>
+        <c:axId val="-849456320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1936,7 +2042,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="531379904"/>
+        <c:crossAx val="-849463392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1944,7 +2050,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="531379904"/>
+        <c:axId val="-849463392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1995,7 +2101,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="531385344"/>
+        <c:crossAx val="-849456320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2135,7 +2241,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$E$5</c:f>
+              <c:f>Feuil1!$F$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2160,7 +2266,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Feuil1!$F$16:$F$19</c:f>
+                <c:f>Feuil1!$G$16:$G$19</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
@@ -2181,7 +2287,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Feuil1!$F$16:$F$19</c:f>
+                <c:f>Feuil1!$G$16:$G$19</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
@@ -2236,7 +2342,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$E$16:$E$19</c:f>
+              <c:f>Feuil1!$F$16:$F$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2266,11 +2372,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="531376640"/>
-        <c:axId val="531377184"/>
+        <c:axId val="-849454144"/>
+        <c:axId val="-849455776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="531376640"/>
+        <c:axId val="-849454144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2313,7 +2419,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="531377184"/>
+        <c:crossAx val="-849455776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2321,7 +2427,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="531377184"/>
+        <c:axId val="-849455776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2372,7 +2478,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="531376640"/>
+        <c:crossAx val="-849454144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2512,7 +2618,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$G$5</c:f>
+              <c:f>Feuil1!$H$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2537,7 +2643,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Feuil1!$H$16:$H$19</c:f>
+                <c:f>Feuil1!$J$16:$J$19</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
@@ -2558,7 +2664,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Feuil1!$H$16:$H$19</c:f>
+                <c:f>Feuil1!$J$16:$J$19</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
@@ -2613,21 +2719,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$G$16:$G$19</c:f>
+              <c:f>Feuil1!$I$16:$I$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.62346824999999995</c:v>
+                  <c:v>0.37653175000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.67698714999999998</c:v>
+                  <c:v>0.32301285000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.58388267500000002</c:v>
+                  <c:v>0.41611732499999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.61082475000000003</c:v>
+                  <c:v>0.38917524999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2643,11 +2749,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="534375984"/>
-        <c:axId val="534374352"/>
+        <c:axId val="-849453056"/>
+        <c:axId val="-849452512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="534375984"/>
+        <c:axId val="-849453056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2690,7 +2796,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="534374352"/>
+        <c:crossAx val="-849452512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2698,7 +2804,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="534374352"/>
+        <c:axId val="-849452512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2749,9 +2855,639 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="534375984"/>
+        <c:crossAx val="-849453056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$F$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Feuil1!$G$20:$G$23</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>1.68108875983272E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.1312804628156001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3.7522838461464099E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.41567846662759E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Feuil1!$G$20:$G$23</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>1.68108875983272E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.1312804628156001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3.7522838461464099E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.41567846662759E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>Feuil1!$E$20:$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$F$20:$F$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.20750004999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21263889999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1825</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19652785</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-776511232"/>
+        <c:axId val="-776519392"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-776511232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-776519392"/>
+        <c:crossesAt val="0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-776519392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-776511232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="5.000000000000001E-2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$H$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Feuil1!$J$20:$J$23</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>4.1375893520873203E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.7998992165374302E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.1438716048784602E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.9529153294700499E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Feuil1!$J$20:$J$23</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>4.1375893520873203E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.7998992165374302E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.1438716048784602E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.9529153294700499E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>Feuil1!$E$20:$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$I$20:$I$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.54514862499999994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.550356925</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.61857965000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.62341457499999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-625292224"/>
+        <c:axId val="-625282976"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-625292224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-625282976"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-625282976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-625292224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3029,6 +3765,83 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -6047,20 +6860,1026 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6081,13 +7900,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>238124</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>685800</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6111,15 +7930,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6143,15 +7962,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>19051</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>133351</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6175,15 +7994,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6207,15 +8026,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>742951</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>57151</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6232,6 +8051,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Graphique 11"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>609601</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Graphique 12"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6503,324 +8386,541 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H19"/>
+  <dimension ref="B3:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="1"/>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="1"/>
+      <c r="F4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="19"/>
+      <c r="H4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="15"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="19"/>
     </row>
-    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="16" t="s">
+    <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="G5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="H5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="I5" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="42" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="52">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6">
         <v>0.1924999</v>
       </c>
-      <c r="F6" s="8">
+      <c r="G6" s="8">
         <v>3.2063951806926803E-2</v>
       </c>
-      <c r="G6" s="6">
+      <c r="H6" s="23">
         <v>0.40652814999999998</v>
       </c>
-      <c r="H6" s="3">
+      <c r="I6" s="29">
+        <f>1-H6</f>
+        <v>0.59347185000000002</v>
+      </c>
+      <c r="J6" s="3">
         <v>4.1544697224981497E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="20" t="s">
+    <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="22"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="53">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2">
         <v>9.0277825000000006E-2</v>
       </c>
-      <c r="F7" s="9">
+      <c r="G7" s="9">
         <v>3.18459590479944E-2</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="24">
         <v>0.30257622499999998</v>
       </c>
-      <c r="H7" s="4">
+      <c r="I7" s="26">
+        <f t="shared" ref="I7:I23" si="0">1-H7</f>
+        <v>0.69742377500000008</v>
+      </c>
+      <c r="J7" s="4">
         <v>3.8694057146886798E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="20" t="s">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="22"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="11">
+        <v>3</v>
+      </c>
+      <c r="F8" s="2">
         <v>0.18708322499999999</v>
       </c>
-      <c r="F8" s="9">
+      <c r="G8" s="9">
         <v>3.9552465277950297E-2</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="24">
         <v>0.43228597499999999</v>
       </c>
-      <c r="H8" s="4">
+      <c r="I8" s="26">
+        <f t="shared" si="0"/>
+        <v>0.56771402500000001</v>
+      </c>
+      <c r="J8" s="4">
         <v>5.6778757277920401E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="12"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="20" t="s">
+    <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="22"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="12">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2">
         <v>0.18569445000000001</v>
       </c>
-      <c r="F9" s="9">
+      <c r="G9" s="9">
         <v>2.8296780036940101E-2</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="24">
         <v>0.39777544999999997</v>
       </c>
-      <c r="H9" s="4">
+      <c r="I9" s="26">
+        <f t="shared" si="0"/>
+        <v>0.60222455000000008</v>
+      </c>
+      <c r="J9" s="4">
         <v>3.62763083836566E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="12"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="20" t="s">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="22"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="11">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2">
         <v>0.20486104999999999</v>
       </c>
-      <c r="F10" s="9">
+      <c r="G10" s="9">
         <v>2.6752897292366299E-2</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="24">
         <v>0.48667115</v>
       </c>
-      <c r="H10" s="4">
+      <c r="I10" s="26">
+        <f t="shared" si="0"/>
+        <v>0.51332884999999995</v>
+      </c>
+      <c r="J10" s="4">
         <v>4.9891727533062397E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="12"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="21" t="s">
+    <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="22"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="13">
+        <v>6</v>
+      </c>
+      <c r="F11" s="7">
         <v>0.1379167</v>
       </c>
-      <c r="F11" s="10">
+      <c r="G11" s="10">
         <v>4.0958140021371298E-2</v>
       </c>
-      <c r="G11" s="7">
+      <c r="H11" s="25">
         <v>0.33149679999999998</v>
       </c>
-      <c r="H11" s="5">
+      <c r="I11" s="30">
+        <f t="shared" si="0"/>
+        <v>0.66850319999999996</v>
+      </c>
+      <c r="J11" s="5">
         <v>3.3580699410257202E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="12"/>
-      <c r="C12" s="25" t="s">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="22"/>
+      <c r="C12" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="11">
+        <v>1</v>
+      </c>
+      <c r="F12" s="6">
         <v>0.19208335000000001</v>
       </c>
-      <c r="F12" s="8">
+      <c r="G12" s="8">
         <v>2.1420261191577101E-2</v>
       </c>
-      <c r="G12" s="6">
+      <c r="H12" s="23">
         <v>0.66134327500000001</v>
       </c>
-      <c r="H12" s="3">
+      <c r="I12" s="29">
+        <f t="shared" si="0"/>
+        <v>0.33865672499999999</v>
+      </c>
+      <c r="J12" s="3">
         <v>7.3376435563814596E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="20" t="s">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="22"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="12">
+        <v>2</v>
+      </c>
+      <c r="F13" s="2">
         <v>0.19916667499999999</v>
       </c>
-      <c r="F13" s="9">
+      <c r="G13" s="9">
         <v>1.8598872493241901E-2</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H13" s="24">
         <v>0.49064137499999999</v>
       </c>
-      <c r="H13" s="4">
+      <c r="I13" s="26">
+        <f t="shared" si="0"/>
+        <v>0.50935862499999995</v>
+      </c>
+      <c r="J13" s="4">
         <v>6.0269449919714703E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="12"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="20" t="s">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="22"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="12">
+        <v>3</v>
+      </c>
+      <c r="F14" s="2">
         <v>0.19388892499999999</v>
       </c>
-      <c r="F14" s="9">
+      <c r="G14" s="9">
         <v>1.9277832625526702E-2</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H14" s="24">
         <v>0.66827780000000003</v>
       </c>
-      <c r="H14" s="4">
+      <c r="I14" s="26">
+        <f t="shared" si="0"/>
+        <v>0.33172219999999997</v>
+      </c>
+      <c r="J14" s="4">
         <v>7.1532251530233695E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="12"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="22" t="s">
+    <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="22"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="15">
+        <v>4</v>
+      </c>
+      <c r="F15" s="7">
         <v>0.205138875</v>
       </c>
-      <c r="F15" s="9">
+      <c r="G15" s="10">
         <v>2.2200427793507602E-2</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="25">
         <v>0.47091192500000001</v>
       </c>
-      <c r="H15" s="4">
+      <c r="I15" s="30">
+        <f t="shared" si="0"/>
+        <v>0.52908807499999999</v>
+      </c>
+      <c r="J15" s="5">
         <v>5.5575377660175701E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="12"/>
-      <c r="C16" s="25" t="s">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="22"/>
+      <c r="C16" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D16" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="14">
+        <v>1</v>
+      </c>
+      <c r="F16" s="6">
         <v>0.1179167</v>
       </c>
-      <c r="F16" s="8">
+      <c r="G16" s="8">
         <v>3.7139850730269097E-2</v>
       </c>
-      <c r="G16" s="6">
+      <c r="H16" s="23">
         <v>0.62346824999999995</v>
       </c>
-      <c r="H16" s="3">
+      <c r="I16" s="29">
+        <f t="shared" si="0"/>
+        <v>0.37653175000000005</v>
+      </c>
+      <c r="J16" s="3">
         <v>0.11158541894538899</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="12"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="24" t="s">
+    <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="22"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="15">
+        <v>2</v>
+      </c>
+      <c r="F17" s="7">
         <v>0.105</v>
       </c>
-      <c r="F17" s="10">
+      <c r="G17" s="10">
         <v>3.3682930733837803E-2</v>
       </c>
-      <c r="G17" s="7">
+      <c r="H17" s="25">
         <v>0.67698714999999998</v>
       </c>
-      <c r="H17" s="5">
+      <c r="I17" s="30">
+        <f t="shared" si="0"/>
+        <v>0.32301285000000002</v>
+      </c>
+      <c r="J17" s="5">
         <v>0.14664725021324199</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="12"/>
-      <c r="C18" s="28" t="s">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="22"/>
+      <c r="C18" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="23" t="s">
+      <c r="D18" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="27">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2">
         <v>0.17680552499999999</v>
       </c>
-      <c r="F18" s="8">
+      <c r="G18" s="9">
         <v>2.6023974797401098E-2</v>
       </c>
-      <c r="G18" s="6">
+      <c r="H18" s="24">
         <v>0.58388267500000002</v>
       </c>
-      <c r="H18" s="3">
+      <c r="I18" s="26">
+        <f t="shared" si="0"/>
+        <v>0.41611732499999998</v>
+      </c>
+      <c r="J18" s="4">
         <v>8.5597527293062303E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="13"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="24" t="s">
+    <row r="19" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="28"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="27">
+        <v>2</v>
+      </c>
+      <c r="F19" s="2">
         <v>0.18888887500000001</v>
       </c>
-      <c r="F19" s="10">
+      <c r="G19" s="9">
         <v>2.02470293372627E-2</v>
       </c>
-      <c r="G19" s="7">
+      <c r="H19" s="24">
         <v>0.61082475000000003</v>
       </c>
-      <c r="H19" s="5">
+      <c r="I19" s="26">
+        <f t="shared" si="0"/>
+        <v>0.38917524999999997</v>
+      </c>
+      <c r="J19" s="4">
         <v>6.8508935964307197E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="14">
+        <v>1</v>
+      </c>
+      <c r="F20" s="29">
+        <v>0.20750004999999999</v>
+      </c>
+      <c r="G20" s="29">
+        <v>1.68108875983272E-2</v>
+      </c>
+      <c r="H20" s="29">
+        <v>0.454851375</v>
+      </c>
+      <c r="I20" s="29">
+        <f t="shared" si="0"/>
+        <v>0.54514862499999994</v>
+      </c>
+      <c r="J20" s="3">
+        <v>4.1375893520873203E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="32"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="27">
+        <v>2</v>
+      </c>
+      <c r="F21" s="26">
+        <v>0.21263889999999999</v>
+      </c>
+      <c r="G21" s="26">
+        <v>2.1312804628156001E-2</v>
+      </c>
+      <c r="H21" s="26">
+        <v>0.449643075</v>
+      </c>
+      <c r="I21" s="26">
+        <f t="shared" si="0"/>
+        <v>0.550356925</v>
+      </c>
+      <c r="J21" s="4">
+        <v>4.7998992165374302E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="32"/>
+      <c r="C22" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="27">
+        <v>3</v>
+      </c>
+      <c r="F22" s="26">
+        <v>0.1825</v>
+      </c>
+      <c r="G22" s="26">
+        <v>3.7522838461464099E-2</v>
+      </c>
+      <c r="H22" s="26">
+        <v>0.38142035000000002</v>
+      </c>
+      <c r="I22" s="26">
+        <f t="shared" si="0"/>
+        <v>0.61857965000000004</v>
+      </c>
+      <c r="J22" s="4">
+        <v>4.1438716048784602E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="33"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="15">
+        <v>4</v>
+      </c>
+      <c r="F23" s="30">
+        <v>0.19652785</v>
+      </c>
+      <c r="G23" s="30">
+        <v>2.41567846662759E-2</v>
+      </c>
+      <c r="H23" s="30">
+        <v>0.37658542499999997</v>
+      </c>
+      <c r="I23" s="30">
+        <f t="shared" si="0"/>
+        <v>0.62341457499999997</v>
+      </c>
+      <c r="J23" s="5">
+        <v>2.9529153294700499E-2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
+  <mergeCells count="10">
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:J4"/>
     <mergeCell ref="B6:B19"/>
     <mergeCell ref="C6:C11"/>
     <mergeCell ref="C12:C15"/>

</xml_diff>